<commit_message>
Add back ALTGX_RECONFIG module (required for Cyclone IV GX). Add BUILDID to PnP ROM.
</commit_message>
<xml_diff>
--- a/ipcores/quartus17.0/kns/PnP_ROM/docs/PnP ROM Structure Definitions.xlsx
+++ b/ipcores/quartus17.0/kns/PnP_ROM/docs/PnP ROM Structure Definitions.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="48">
   <si>
     <t>00h</t>
   </si>
@@ -162,6 +162,9 @@
   </si>
   <si>
     <t>Git Commit</t>
+  </si>
+  <si>
+    <t>Build ID (Unix Time)</t>
   </si>
 </sst>
 </file>
@@ -419,15 +422,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -444,6 +438,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1327,39 +1330,43 @@
       </c>
     </row>
     <row r="13" spans="1:33" s="4" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="6"/>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="6"/>
-      <c r="J13" s="6"/>
-      <c r="K13" s="6"/>
-      <c r="L13" s="6"/>
-      <c r="M13" s="6"/>
-      <c r="N13" s="6"/>
-      <c r="O13" s="6"/>
-      <c r="P13" s="6"/>
-      <c r="Q13" s="6"/>
-      <c r="R13" s="6"/>
-      <c r="S13" s="6"/>
-      <c r="T13" s="6"/>
-      <c r="U13" s="6"/>
-      <c r="V13" s="6"/>
-      <c r="W13" s="6"/>
-      <c r="X13" s="6"/>
-      <c r="Y13" s="6"/>
-      <c r="Z13" s="6"/>
-      <c r="AA13" s="6"/>
-      <c r="AB13" s="6"/>
-      <c r="AC13" s="6"/>
-      <c r="AD13" s="6"/>
-      <c r="AE13" s="6"/>
-      <c r="AF13" s="6"/>
-      <c r="AG13" s="11"/>
+      <c r="A13" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="B13" s="21"/>
+      <c r="C13" s="21"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="21"/>
+      <c r="F13" s="21"/>
+      <c r="G13" s="21"/>
+      <c r="H13" s="21"/>
+      <c r="I13" s="21"/>
+      <c r="J13" s="21"/>
+      <c r="K13" s="21"/>
+      <c r="L13" s="21"/>
+      <c r="M13" s="21"/>
+      <c r="N13" s="21"/>
+      <c r="O13" s="21"/>
+      <c r="P13" s="21"/>
+      <c r="Q13" s="21"/>
+      <c r="R13" s="21"/>
+      <c r="S13" s="21"/>
+      <c r="T13" s="21"/>
+      <c r="U13" s="21"/>
+      <c r="V13" s="21"/>
+      <c r="W13" s="21"/>
+      <c r="X13" s="21"/>
+      <c r="Y13" s="21"/>
+      <c r="Z13" s="21"/>
+      <c r="AA13" s="21"/>
+      <c r="AB13" s="21"/>
+      <c r="AC13" s="21"/>
+      <c r="AD13" s="21"/>
+      <c r="AE13" s="21"/>
+      <c r="AF13" s="22"/>
+      <c r="AG13" s="5" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="14" spans="1:33" s="4" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>
@@ -1747,7 +1754,15 @@
       <c r="AG24" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="15">
+  <mergeCells count="16">
+    <mergeCell ref="A13:AF13"/>
+    <mergeCell ref="A5:P5"/>
+    <mergeCell ref="Q5:AF5"/>
+    <mergeCell ref="A3:P3"/>
+    <mergeCell ref="Q3:T3"/>
+    <mergeCell ref="U3:AF3"/>
+    <mergeCell ref="A4:P4"/>
+    <mergeCell ref="Q4:AF4"/>
     <mergeCell ref="A11:P11"/>
     <mergeCell ref="Q11:AF11"/>
     <mergeCell ref="A12:AF12"/>
@@ -1756,13 +1771,6 @@
     <mergeCell ref="U9:AF9"/>
     <mergeCell ref="A10:P10"/>
     <mergeCell ref="Q10:AF10"/>
-    <mergeCell ref="A5:P5"/>
-    <mergeCell ref="Q5:AF5"/>
-    <mergeCell ref="A3:P3"/>
-    <mergeCell ref="Q3:T3"/>
-    <mergeCell ref="U3:AF3"/>
-    <mergeCell ref="A4:P4"/>
-    <mergeCell ref="Q4:AF4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -2882,42 +2890,42 @@
       </c>
     </row>
     <row r="4" spans="1:33" s="4" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="29" t="s">
+      <c r="A4" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="B4" s="30"/>
-      <c r="C4" s="30"/>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="30"/>
-      <c r="G4" s="30"/>
-      <c r="H4" s="30"/>
-      <c r="I4" s="30"/>
-      <c r="J4" s="30"/>
-      <c r="K4" s="30"/>
-      <c r="L4" s="30"/>
-      <c r="M4" s="30"/>
-      <c r="N4" s="30"/>
-      <c r="O4" s="30"/>
-      <c r="P4" s="31"/>
-      <c r="Q4" s="26" t="s">
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="27"/>
+      <c r="J4" s="27"/>
+      <c r="K4" s="27"/>
+      <c r="L4" s="27"/>
+      <c r="M4" s="27"/>
+      <c r="N4" s="27"/>
+      <c r="O4" s="27"/>
+      <c r="P4" s="28"/>
+      <c r="Q4" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="R4" s="27"/>
-      <c r="S4" s="27"/>
-      <c r="T4" s="27"/>
-      <c r="U4" s="27"/>
-      <c r="V4" s="27"/>
-      <c r="W4" s="27"/>
-      <c r="X4" s="27"/>
-      <c r="Y4" s="27"/>
-      <c r="Z4" s="27"/>
-      <c r="AA4" s="27"/>
-      <c r="AB4" s="27"/>
-      <c r="AC4" s="27"/>
-      <c r="AD4" s="27"/>
-      <c r="AE4" s="27"/>
-      <c r="AF4" s="28"/>
+      <c r="R4" s="24"/>
+      <c r="S4" s="24"/>
+      <c r="T4" s="24"/>
+      <c r="U4" s="24"/>
+      <c r="V4" s="24"/>
+      <c r="W4" s="24"/>
+      <c r="X4" s="24"/>
+      <c r="Y4" s="24"/>
+      <c r="Z4" s="24"/>
+      <c r="AA4" s="24"/>
+      <c r="AB4" s="24"/>
+      <c r="AC4" s="24"/>
+      <c r="AD4" s="24"/>
+      <c r="AE4" s="24"/>
+      <c r="AF4" s="25"/>
       <c r="AG4" s="5" t="s">
         <v>3</v>
       </c>
@@ -2933,16 +2941,16 @@
       <c r="F5" s="21"/>
       <c r="G5" s="21"/>
       <c r="H5" s="22"/>
-      <c r="I5" s="23" t="s">
+      <c r="I5" s="31" t="s">
         <v>40</v>
       </c>
-      <c r="J5" s="23"/>
-      <c r="K5" s="23"/>
-      <c r="L5" s="23"/>
-      <c r="M5" s="23"/>
-      <c r="N5" s="23"/>
-      <c r="O5" s="23"/>
-      <c r="P5" s="23"/>
+      <c r="J5" s="31"/>
+      <c r="K5" s="31"/>
+      <c r="L5" s="31"/>
+      <c r="M5" s="31"/>
+      <c r="N5" s="31"/>
+      <c r="O5" s="31"/>
+      <c r="P5" s="31"/>
       <c r="Q5" s="17" t="s">
         <v>41</v>
       </c>
@@ -3201,21 +3209,21 @@
       <c r="Q10" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="R10" s="24"/>
-      <c r="S10" s="24"/>
-      <c r="T10" s="24"/>
-      <c r="U10" s="24"/>
-      <c r="V10" s="24"/>
-      <c r="W10" s="24"/>
-      <c r="X10" s="24"/>
-      <c r="Y10" s="24"/>
-      <c r="Z10" s="24"/>
-      <c r="AA10" s="24"/>
-      <c r="AB10" s="24"/>
-      <c r="AC10" s="24"/>
-      <c r="AD10" s="24"/>
-      <c r="AE10" s="24"/>
-      <c r="AF10" s="25"/>
+      <c r="R10" s="29"/>
+      <c r="S10" s="29"/>
+      <c r="T10" s="29"/>
+      <c r="U10" s="29"/>
+      <c r="V10" s="29"/>
+      <c r="W10" s="29"/>
+      <c r="X10" s="29"/>
+      <c r="Y10" s="29"/>
+      <c r="Z10" s="29"/>
+      <c r="AA10" s="29"/>
+      <c r="AB10" s="29"/>
+      <c r="AC10" s="29"/>
+      <c r="AD10" s="29"/>
+      <c r="AE10" s="29"/>
+      <c r="AF10" s="30"/>
       <c r="AG10" s="5" t="s">
         <v>3</v>
       </c>
@@ -3387,16 +3395,16 @@
       <c r="F15" s="21"/>
       <c r="G15" s="21"/>
       <c r="H15" s="22"/>
-      <c r="I15" s="23" t="s">
+      <c r="I15" s="31" t="s">
         <v>40</v>
       </c>
-      <c r="J15" s="23"/>
-      <c r="K15" s="23"/>
-      <c r="L15" s="23"/>
-      <c r="M15" s="23"/>
-      <c r="N15" s="23"/>
-      <c r="O15" s="23"/>
-      <c r="P15" s="23"/>
+      <c r="J15" s="31"/>
+      <c r="K15" s="31"/>
+      <c r="L15" s="31"/>
+      <c r="M15" s="31"/>
+      <c r="N15" s="31"/>
+      <c r="O15" s="31"/>
+      <c r="P15" s="31"/>
       <c r="Q15" s="17" t="s">
         <v>41</v>
       </c>
@@ -3862,24 +3870,24 @@
       <c r="N26" s="21"/>
       <c r="O26" s="21"/>
       <c r="P26" s="22"/>
-      <c r="Q26" s="24" t="s">
+      <c r="Q26" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="R26" s="24"/>
-      <c r="S26" s="24"/>
-      <c r="T26" s="24"/>
-      <c r="U26" s="24"/>
-      <c r="V26" s="24"/>
-      <c r="W26" s="24"/>
-      <c r="X26" s="24"/>
-      <c r="Y26" s="24"/>
-      <c r="Z26" s="24"/>
-      <c r="AA26" s="24"/>
-      <c r="AB26" s="24"/>
-      <c r="AC26" s="24"/>
-      <c r="AD26" s="24"/>
-      <c r="AE26" s="24"/>
-      <c r="AF26" s="25"/>
+      <c r="R26" s="29"/>
+      <c r="S26" s="29"/>
+      <c r="T26" s="29"/>
+      <c r="U26" s="29"/>
+      <c r="V26" s="29"/>
+      <c r="W26" s="29"/>
+      <c r="X26" s="29"/>
+      <c r="Y26" s="29"/>
+      <c r="Z26" s="29"/>
+      <c r="AA26" s="29"/>
+      <c r="AB26" s="29"/>
+      <c r="AC26" s="29"/>
+      <c r="AD26" s="29"/>
+      <c r="AE26" s="29"/>
+      <c r="AF26" s="30"/>
       <c r="AG26" s="5" t="s">
         <v>3</v>
       </c>
@@ -4499,24 +4507,6 @@
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="A3:P3"/>
-    <mergeCell ref="Q4:AF4"/>
-    <mergeCell ref="Q3:T3"/>
-    <mergeCell ref="U3:AF3"/>
-    <mergeCell ref="A4:P4"/>
-    <mergeCell ref="A25:P25"/>
-    <mergeCell ref="Q25:T25"/>
-    <mergeCell ref="U25:AF25"/>
-    <mergeCell ref="A32:P32"/>
-    <mergeCell ref="AC32:AF32"/>
-    <mergeCell ref="Q32:AB32"/>
-    <mergeCell ref="Q26:AF26"/>
-    <mergeCell ref="A26:P26"/>
-    <mergeCell ref="A31:P31"/>
-    <mergeCell ref="Q31:AF31"/>
-    <mergeCell ref="A30:P30"/>
-    <mergeCell ref="Q30:T30"/>
-    <mergeCell ref="U30:AF30"/>
     <mergeCell ref="A15:H15"/>
     <mergeCell ref="I15:P15"/>
     <mergeCell ref="Q15:AF15"/>
@@ -4532,6 +4522,24 @@
     <mergeCell ref="A12:AF12"/>
     <mergeCell ref="A13:AF13"/>
     <mergeCell ref="A14:AF14"/>
+    <mergeCell ref="A25:P25"/>
+    <mergeCell ref="Q25:T25"/>
+    <mergeCell ref="U25:AF25"/>
+    <mergeCell ref="A32:P32"/>
+    <mergeCell ref="AC32:AF32"/>
+    <mergeCell ref="Q32:AB32"/>
+    <mergeCell ref="Q26:AF26"/>
+    <mergeCell ref="A26:P26"/>
+    <mergeCell ref="A31:P31"/>
+    <mergeCell ref="Q31:AF31"/>
+    <mergeCell ref="A30:P30"/>
+    <mergeCell ref="Q30:T30"/>
+    <mergeCell ref="U30:AF30"/>
+    <mergeCell ref="A3:P3"/>
+    <mergeCell ref="Q4:AF4"/>
+    <mergeCell ref="Q3:T3"/>
+    <mergeCell ref="U3:AF3"/>
+    <mergeCell ref="A4:P4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" verticalDpi="0" r:id="rId1"/>

</xml_diff>